<commit_message>
Failing test added for plane initialising with airport property
</commit_message>
<xml_diff>
--- a/Airport Challenge - Domain Model.xlsx
+++ b/Airport Challenge - Domain Model.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -48,6 +48,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- constructor</t>
     </r>
@@ -57,6 +58,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -65,6 +67,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@String</t>
     </r>
@@ -74,6 +77,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -102,6 +106,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-landPlane</t>
     </r>
@@ -111,6 +116,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -119,6 +125,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@Plane</t>
     </r>
@@ -128,6 +135,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -150,6 +158,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- name </t>
     </r>
@@ -159,6 +168,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -167,6 +177,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@String</t>
     </r>
@@ -176,6 +187,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -186,6 +198,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- capacity </t>
     </r>
@@ -195,6 +208,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -203,6 +217,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@Number</t>
     </r>
@@ -212,6 +227,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -228,6 +244,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-changeCapacity</t>
     </r>
@@ -237,6 +254,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -245,6 +263,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@Number</t>
     </r>
@@ -254,6 +273,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -267,6 +287,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- planes </t>
     </r>
@@ -276,6 +297,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -284,6 +306,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@Array</t>
     </r>
@@ -293,6 +316,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -309,6 +333,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- landPlane</t>
     </r>
@@ -318,6 +343,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -326,6 +352,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">@Plane</t>
     </r>
@@ -335,6 +362,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -361,6 +389,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -382,18 +411,21 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -474,14 +506,14 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.78"/>
   </cols>
@@ -627,8 +659,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Failing test added for airport changeCapacity method
</commit_message>
<xml_diff>
--- a/Airport Challenge - Domain Model.xlsx
+++ b/Airport Challenge - Domain Model.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">Airport Challenge – Week 1</t>
   </si>
@@ -279,7 +279,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">@Number “new capacity”</t>
+    <t xml:space="preserve">@String “capacity change to newCapacity”</t>
   </si>
   <si>
     <r>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t xml:space="preserve">@String “Plane ___ has taken off from airport ____.” / “This plane is not at this airport, cannot take off.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extended Acceptance criteria</t>
   </si>
 </sst>
 </file>
@@ -504,13 +507,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.89"/>
@@ -654,6 +657,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Failing test added for airport planes property. Exports simplified
</commit_message>
<xml_diff>
--- a/Airport Challenge - Domain Model.xlsx
+++ b/Airport Challenge - Domain Model.xlsx
@@ -279,7 +279,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">@String “capacity change to newCapacity”</t>
+    <t xml:space="preserve">log “capacity changed to newCapacity”</t>
   </si>
   <si>
     <r>
@@ -368,13 +368,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">@String “Plane ___ landed successfully.” / “Airport is full, cannot land.” / “This plane is already at this airport, cannot re-land.”</t>
+    <t xml:space="preserve">Log / @Error “Plane ___ landed successfully.” / “Airport is full, cannot land.” / “This plane is already at this airport, cannot re-land.”</t>
   </si>
   <si>
     <t xml:space="preserve">- takeOffPlane(@Plane)</t>
   </si>
   <si>
-    <t xml:space="preserve">@String “Plane ___ has taken off from airport ____.” / “This plane is not at this airport, cannot take off.”</t>
+    <t xml:space="preserve">Log / @Error “Plane ___ has taken off from airport ____.” / “This plane is not at this airport, cannot take off.”</t>
   </si>
   <si>
     <t xml:space="preserve">Extended Acceptance criteria</t>
@@ -510,7 +510,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Tests added for returning plane object when land/takeoff
</commit_message>
<xml_diff>
--- a/Airport Challenge - Domain Model.xlsx
+++ b/Airport Challenge - Domain Model.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t xml:space="preserve">Airport Challenge – Week 1</t>
   </si>
@@ -368,13 +368,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Log / @Error “Plane ___ landed successfully.” / “Airport is full, cannot land.” / “This plane is already at this airport, cannot re-land.”</t>
+    <t xml:space="preserve">Log / @Error / return: “Plane ___ landed successfully.” / “Airport is full, cannot land.” / “This plane is already at this airport, cannot re-land.”</t>
   </si>
   <si>
     <t xml:space="preserve">- takeOffPlane(@Plane)</t>
   </si>
   <si>
-    <t xml:space="preserve">Log / @Error “Plane ___ has taken off from airport ____.” / “This plane is not at this airport, cannot take off.”</t>
+    <t xml:space="preserve">Log / @Error / return: “Plane ___ has taken off from airport ____.” / “This plane is not at this airport, cannot take off.”</t>
   </si>
   <si>
     <t xml:space="preserve">Extended Acceptance criteria</t>
@@ -507,18 +507,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,6 +649,9 @@
       <c r="D18" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="L18" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
@@ -655,6 +659,9 @@
       </c>
       <c r="D19" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>